<commit_message>
Update binary files after adding to sharepoint synched folder.
</commit_message>
<xml_diff>
--- a/R/EXCEL/Split files with R - Data Group 4-22-2020/Output files/output_BAR01.xlsx
+++ b/R/EXCEL/Split files with R - Data Group 4-22-2020/Output files/output_BAR01.xlsx
@@ -7956,4 +7956,169 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F037E4F129E6AB4FAC70B4DD2DC11BE8" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34b0eef908b8cb47995c0fb33ea54a2f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="301009bb-228e-4156-8800-44dd3ce9088c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5eb22e3a97bd65c4e8fa7bbcc64484de" ns2:_="">
+    <xsd:import namespace="301009bb-228e-4156-8800-44dd3ce9088c"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="301009bb-228e-4156-8800-44dd3ce9088c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52B9631F-5778-48B5-B779-93F171963858}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC626CC-980A-4C5B-A534-F261ADCD29D6}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E19C62C-E20D-4A69-A75C-07436E457DF0}"/>
 </file>
</xml_diff>

<commit_message>
Revert "Update binary files after adding to sharepoint synched folder."
This reverts commit a86556bf7e0d66220c9eb1f6d29bf331b67aae80.
</commit_message>
<xml_diff>
--- a/R/EXCEL/Split files with R - Data Group 4-22-2020/Output files/output_BAR01.xlsx
+++ b/R/EXCEL/Split files with R - Data Group 4-22-2020/Output files/output_BAR01.xlsx
@@ -7956,169 +7956,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F037E4F129E6AB4FAC70B4DD2DC11BE8" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34b0eef908b8cb47995c0fb33ea54a2f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="301009bb-228e-4156-8800-44dd3ce9088c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5eb22e3a97bd65c4e8fa7bbcc64484de" ns2:_="">
-    <xsd:import namespace="301009bb-228e-4156-8800-44dd3ce9088c"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="301009bb-228e-4156-8800-44dd3ce9088c" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52B9631F-5778-48B5-B779-93F171963858}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBC626CC-980A-4C5B-A534-F261ADCD29D6}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E19C62C-E20D-4A69-A75C-07436E457DF0}"/>
 </file>
</xml_diff>